<commit_message>
update smaller data exports
</commit_message>
<xml_diff>
--- a/data-export/export_202204/sum_tagged_all_ops.xlsx
+++ b/data-export/export_202204/sum_tagged_all_ops.xlsx
@@ -438,16 +438,16 @@
         <v>83310636910.11037</v>
       </c>
       <c r="F2">
-        <v>142257627807.7419</v>
+        <v>142408862489.6619</v>
       </c>
       <c r="G2">
-        <v>123364078225.058</v>
+        <v>123470149677.878</v>
       </c>
       <c r="H2">
-        <v>16656197954.84388</v>
+        <v>16701310436.44388</v>
       </c>
       <c r="I2">
-        <v>2237351627.84</v>
+        <v>2237402375.34</v>
       </c>
       <c r="J2">
         <v>10628213704.66506</v>
@@ -715,16 +715,16 @@
         <v>84069139683.82854</v>
       </c>
       <c r="F9">
-        <v>142603867584.6269</v>
+        <v>142625904398.2969</v>
       </c>
       <c r="G9">
-        <v>67327399355.61</v>
+        <v>67349336169.53</v>
       </c>
       <c r="H9">
         <v>1327735458.67</v>
       </c>
       <c r="I9">
-        <v>73948732770.34695</v>
+        <v>73948832770.09695</v>
       </c>
       <c r="J9">
         <v>405580444.3399999</v>
@@ -1069,13 +1069,13 @@
         <v>69199503348.10663</v>
       </c>
       <c r="F18">
-        <v>97135407978.82335</v>
+        <v>97147960741.49001</v>
       </c>
       <c r="G18">
-        <v>78293238712.0183</v>
+        <v>78302924392.54497</v>
       </c>
       <c r="H18">
-        <v>17026569450.585</v>
+        <v>17029436532.725</v>
       </c>
       <c r="I18">
         <v>1815599816.22</v>
@@ -1106,13 +1106,13 @@
         <v>9674159.83333333</v>
       </c>
       <c r="F19">
-        <v>342623456.1066667</v>
+        <v>360958057.4400001</v>
       </c>
       <c r="G19">
-        <v>241656689.7916667</v>
+        <v>255795847.375</v>
       </c>
       <c r="H19">
-        <v>100966766.315</v>
+        <v>105162210.065</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -1263,10 +1263,10 @@
         <v>24703655647.15</v>
       </c>
       <c r="F23">
-        <v>35301617284.35</v>
+        <v>35301809979.14999</v>
       </c>
       <c r="G23">
-        <v>29820667005.6</v>
+        <v>29820859700.4</v>
       </c>
       <c r="H23">
         <v>1958111917.28</v>

</xml_diff>